<commit_message>
feat: add MFRD and AFRD metrics to evaluation framework
</commit_message>
<xml_diff>
--- a/results/20250528/evaluation_CHD_49_noisy_0.0.xlsx
+++ b/results/20250528/evaluation_CHD_49_noisy_0.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="35">
   <si>
     <t>Base_Learner</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>cv_ir</t>
+  </si>
+  <si>
+    <t>mfrd</t>
+  </si>
+  <si>
+    <t>afrd</t>
   </si>
   <si>
     <t>hamming_accuracy_PRE_ORDER</t>
@@ -470,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -640,14 +646,11 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
@@ -655,13 +658,13 @@
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H7">
-        <v>0.69524</v>
+        <v>0.99814</v>
       </c>
       <c r="I7">
-        <v>0.02378</v>
+        <v>0.00186</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -669,14 +672,11 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
@@ -684,13 +684,13 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H8">
-        <v>0.14778</v>
+        <v>0.54075</v>
       </c>
       <c r="I8">
-        <v>0.01828</v>
+        <v>0.03146</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -713,13 +713,13 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H9">
-        <v>0.61757</v>
+        <v>0.69524</v>
       </c>
       <c r="I9">
-        <v>0.03911</v>
+        <v>0.02378</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -742,13 +742,13 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H10">
-        <v>5.86518</v>
+        <v>0.14778</v>
       </c>
       <c r="I10">
-        <v>0.81819</v>
+        <v>0.01828</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -771,13 +771,13 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H11">
-        <v>1.75366</v>
+        <v>0.61757</v>
       </c>
       <c r="I11">
-        <v>0.05232</v>
+        <v>0.03911</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -785,10 +785,13 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -797,13 +800,13 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H12">
-        <v>0.6916099999999999</v>
+        <v>5.86518</v>
       </c>
       <c r="I12">
-        <v>0.009950000000000001</v>
+        <v>0.81819</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -811,10 +814,13 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
@@ -823,13 +829,13 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H13">
-        <v>0.15857</v>
+        <v>1.75366</v>
       </c>
       <c r="I13">
-        <v>0.00389</v>
+        <v>0.05232</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -837,10 +843,13 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
@@ -849,13 +858,13 @@
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H14">
-        <v>0.6522</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>0.01779</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -863,10 +872,13 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
@@ -875,13 +887,13 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H15">
-        <v>5.86518</v>
+        <v>0.63222</v>
       </c>
       <c r="I15">
-        <v>0.81819</v>
+        <v>0.11387</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -901,13 +913,13 @@
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H16">
-        <v>1.75366</v>
+        <v>0.6916099999999999</v>
       </c>
       <c r="I16">
-        <v>0.05232</v>
+        <v>0.009950000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -915,14 +927,11 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
@@ -930,13 +939,13 @@
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H17">
-        <v>0.68863</v>
+        <v>0.15857</v>
       </c>
       <c r="I17">
-        <v>0.02557</v>
+        <v>0.00389</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -944,14 +953,11 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
@@ -959,13 +965,13 @@
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H18">
-        <v>0.13341</v>
+        <v>0.6522</v>
       </c>
       <c r="I18">
-        <v>0.03988</v>
+        <v>0.01779</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -973,14 +979,11 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
@@ -988,13 +991,13 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H19">
-        <v>0.60093</v>
+        <v>5.86518</v>
       </c>
       <c r="I19">
-        <v>0.04503</v>
+        <v>0.81819</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1002,14 +1005,11 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
@@ -1017,13 +1017,13 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H20">
-        <v>5.86518</v>
+        <v>1.75366</v>
       </c>
       <c r="I20">
-        <v>0.81819</v>
+        <v>0.05232</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1031,14 +1031,11 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
       <c r="E21" t="s">
         <v>20</v>
       </c>
@@ -1046,13 +1043,13 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H21">
-        <v>1.75366</v>
+        <v>0.99814</v>
       </c>
       <c r="I21">
-        <v>0.05232</v>
+        <v>0.00186</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1060,25 +1057,25 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H22">
-        <v>0.69071</v>
+        <v>0.54235</v>
       </c>
       <c r="I22">
-        <v>0.01326</v>
+        <v>0.03265</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1086,25 +1083,28 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23">
-        <v>0.17119</v>
+        <v>0.68863</v>
       </c>
       <c r="I23">
-        <v>0.01292</v>
+        <v>0.02557</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1112,25 +1112,28 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24" t="s">
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24">
-        <v>0.65604</v>
+        <v>0.13341</v>
       </c>
       <c r="I24">
-        <v>0.01831</v>
+        <v>0.03988</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1138,25 +1141,28 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" t="s">
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25">
-        <v>5.86518</v>
+        <v>0.60093</v>
       </c>
       <c r="I25">
-        <v>0.81819</v>
+        <v>0.04503</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1164,25 +1170,28 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F26" t="s">
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H26">
-        <v>1.75366</v>
+        <v>5.86518</v>
       </c>
       <c r="I26">
-        <v>0.05232</v>
+        <v>0.81819</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1190,28 +1199,28 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F27" t="s">
         <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H27">
-        <v>0.69042</v>
+        <v>1.75366</v>
       </c>
       <c r="I27">
-        <v>0.01596</v>
+        <v>0.05232</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1219,28 +1228,28 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F28" t="s">
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H28">
-        <v>0.16938</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>0.00391</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1248,28 +1257,28 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F29" t="s">
         <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H29">
-        <v>0.64991</v>
+        <v>0.6616300000000001</v>
       </c>
       <c r="I29">
-        <v>0.02123</v>
+        <v>0.10172</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1277,14 +1286,11 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
       </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
       <c r="E30" t="s">
         <v>21</v>
       </c>
@@ -1292,13 +1298,13 @@
         <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H30">
-        <v>5.86518</v>
+        <v>0.69071</v>
       </c>
       <c r="I30">
-        <v>0.81819</v>
+        <v>0.01326</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1306,14 +1312,11 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
       <c r="E31" t="s">
         <v>21</v>
       </c>
@@ -1321,13 +1324,13 @@
         <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H31">
-        <v>1.75366</v>
+        <v>0.17119</v>
       </c>
       <c r="I31">
-        <v>0.05232</v>
+        <v>0.01292</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1335,10 +1338,10 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E32" t="s">
         <v>21</v>
@@ -1347,13 +1350,13 @@
         <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H32">
-        <v>0.69101</v>
+        <v>0.65604</v>
       </c>
       <c r="I32">
-        <v>0.01296</v>
+        <v>0.01831</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1361,10 +1364,10 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E33" t="s">
         <v>21</v>
@@ -1373,13 +1376,13 @@
         <v>22</v>
       </c>
       <c r="G33" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H33">
-        <v>0.16939</v>
+        <v>5.86518</v>
       </c>
       <c r="I33">
-        <v>0.01112</v>
+        <v>0.81819</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1387,10 +1390,10 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E34" t="s">
         <v>21</v>
@@ -1399,13 +1402,13 @@
         <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H34">
-        <v>0.6562</v>
+        <v>1.75366</v>
       </c>
       <c r="I34">
-        <v>0.01799</v>
+        <v>0.05232</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1413,10 +1416,10 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E35" t="s">
         <v>21</v>
@@ -1425,13 +1428,13 @@
         <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H35">
-        <v>5.86518</v>
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>0.81819</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1439,10 +1442,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E36" t="s">
         <v>21</v>
@@ -1451,13 +1454,13 @@
         <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H36">
-        <v>1.75366</v>
+        <v>0.59209</v>
       </c>
       <c r="I36">
-        <v>0.05232</v>
+        <v>0.02609</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1465,10 +1468,10 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -1483,10 +1486,10 @@
         <v>24</v>
       </c>
       <c r="H37">
-        <v>0.68891</v>
+        <v>0.69042</v>
       </c>
       <c r="I37">
-        <v>0.01445</v>
+        <v>0.01596</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1494,10 +1497,10 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -1512,10 +1515,10 @@
         <v>25</v>
       </c>
       <c r="H38">
-        <v>0.16577</v>
+        <v>0.16938</v>
       </c>
       <c r="I38">
-        <v>0.0003</v>
+        <v>0.00391</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1523,10 +1526,10 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -1541,10 +1544,10 @@
         <v>26</v>
       </c>
       <c r="H39">
-        <v>0.6483100000000001</v>
+        <v>0.64991</v>
       </c>
       <c r="I39">
-        <v>0.01939</v>
+        <v>0.02123</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1552,10 +1555,10 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40">
         <v>2</v>
@@ -1581,10 +1584,10 @@
         <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -1610,25 +1613,28 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
       </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G42" t="s">
         <v>29</v>
       </c>
       <c r="H42">
-        <v>0.50238</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>0.01868</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1636,25 +1642,28 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
       </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G43" t="s">
         <v>30</v>
       </c>
       <c r="H43">
-        <v>0.09186999999999999</v>
+        <v>0.59173</v>
       </c>
       <c r="I43">
-        <v>0.01245</v>
+        <v>0.02071</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1662,28 +1671,25 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E44" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H44">
-        <v>0.45301</v>
+        <v>0.69101</v>
       </c>
       <c r="I44">
-        <v>0.02256</v>
+        <v>0.01296</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1691,28 +1697,25 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E45" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G45" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>0.16939</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>0.01112</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1720,25 +1723,25 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
       </c>
       <c r="E46" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H46">
-        <v>0.50273</v>
+        <v>0.6562</v>
       </c>
       <c r="I46">
-        <v>0.01448</v>
+        <v>0.01799</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1746,25 +1749,25 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
         <v>19</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H47">
-        <v>0.09365999999999999</v>
+        <v>5.86518</v>
       </c>
       <c r="I47">
-        <v>0.02145</v>
+        <v>0.81819</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1772,28 +1775,25 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
       </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
       <c r="E48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H48">
-        <v>0.45062</v>
+        <v>1.75366</v>
       </c>
       <c r="I48">
-        <v>0.0264</v>
+        <v>0.05232</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1801,25 +1801,22 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C49" t="s">
         <v>19</v>
       </c>
-      <c r="D49">
-        <v>2</v>
-      </c>
       <c r="E49" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -1830,25 +1827,25 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E50" t="s">
         <v>21</v>
       </c>
       <c r="F50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H50">
-        <v>0.56842</v>
+        <v>0.58905</v>
       </c>
       <c r="I50">
-        <v>0.00607</v>
+        <v>0.02305</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1856,25 +1853,28 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
       </c>
       <c r="E51" t="s">
         <v>21</v>
       </c>
       <c r="F51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G51" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H51">
-        <v>0.03061</v>
+        <v>0.68891</v>
       </c>
       <c r="I51">
-        <v>0.00895</v>
+        <v>0.01445</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1882,10 +1882,10 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -1894,16 +1894,16 @@
         <v>21</v>
       </c>
       <c r="F52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G52" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H52">
-        <v>0.56915</v>
+        <v>0.16577</v>
       </c>
       <c r="I52">
-        <v>0.009429999999999999</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1911,10 +1911,10 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -1923,16 +1923,16 @@
         <v>21</v>
       </c>
       <c r="F53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G53" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H53">
-        <v>0.03242</v>
+        <v>0.6483100000000001</v>
       </c>
       <c r="I53">
-        <v>0.00715</v>
+        <v>0.01939</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -1940,25 +1940,28 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
         <v>19</v>
       </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
       <c r="E54" t="s">
         <v>21</v>
       </c>
       <c r="F54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G54" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H54">
-        <v>0.56902</v>
+        <v>5.86518</v>
       </c>
       <c r="I54">
-        <v>0.00619</v>
+        <v>0.81819</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1966,25 +1969,28 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
         <v>19</v>
       </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
       <c r="E55" t="s">
         <v>21</v>
       </c>
       <c r="F55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H55">
-        <v>0.03061</v>
+        <v>1.75366</v>
       </c>
       <c r="I55">
-        <v>0.00895</v>
+        <v>0.05232</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2004,16 +2010,16 @@
         <v>21</v>
       </c>
       <c r="F56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H56">
-        <v>0.5683</v>
+        <v>1</v>
       </c>
       <c r="I56">
-        <v>0.00787</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2033,15 +2039,455 @@
         <v>21</v>
       </c>
       <c r="F57" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H57">
+        <v>0.58891</v>
+      </c>
+      <c r="I57">
+        <v>0.02065</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" t="s">
         <v>23</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58">
+        <v>0.50238</v>
+      </c>
+      <c r="I58">
+        <v>0.01868</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" t="s">
         <v>32</v>
       </c>
-      <c r="H57">
+      <c r="H59">
+        <v>0.09186999999999999</v>
+      </c>
+      <c r="I59">
+        <v>0.01245</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" t="s">
+        <v>31</v>
+      </c>
+      <c r="H60">
+        <v>0.45301</v>
+      </c>
+      <c r="I60">
+        <v>0.02256</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>32</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" t="s">
+        <v>31</v>
+      </c>
+      <c r="H62">
+        <v>0.50273</v>
+      </c>
+      <c r="I62">
+        <v>0.01448</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63">
+        <v>0.09365999999999999</v>
+      </c>
+      <c r="I63">
+        <v>0.02145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" t="s">
+        <v>23</v>
+      </c>
+      <c r="G64" t="s">
+        <v>31</v>
+      </c>
+      <c r="H64">
+        <v>0.45062</v>
+      </c>
+      <c r="I64">
+        <v>0.0264</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" t="s">
+        <v>32</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" t="s">
+        <v>21</v>
+      </c>
+      <c r="F66" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" t="s">
+        <v>33</v>
+      </c>
+      <c r="H66">
+        <v>0.56842</v>
+      </c>
+      <c r="I66">
+        <v>0.00607</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" t="s">
+        <v>21</v>
+      </c>
+      <c r="F67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67">
+        <v>0.03061</v>
+      </c>
+      <c r="I67">
+        <v>0.00895</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>21</v>
+      </c>
+      <c r="F68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" t="s">
+        <v>33</v>
+      </c>
+      <c r="H68">
+        <v>0.56915</v>
+      </c>
+      <c r="I68">
+        <v>0.009429999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>21</v>
+      </c>
+      <c r="F69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H69">
         <v>0.03242</v>
       </c>
-      <c r="I57">
+      <c r="I69">
+        <v>0.00715</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" t="s">
+        <v>21</v>
+      </c>
+      <c r="F70" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H70">
+        <v>0.56902</v>
+      </c>
+      <c r="I70">
+        <v>0.00619</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" t="s">
+        <v>34</v>
+      </c>
+      <c r="H71">
+        <v>0.03061</v>
+      </c>
+      <c r="I71">
+        <v>0.00895</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>9</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" t="s">
+        <v>33</v>
+      </c>
+      <c r="H72">
+        <v>0.5683</v>
+      </c>
+      <c r="I72">
+        <v>0.00787</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73" t="s">
+        <v>21</v>
+      </c>
+      <c r="F73" t="s">
+        <v>23</v>
+      </c>
+      <c r="G73" t="s">
+        <v>34</v>
+      </c>
+      <c r="H73">
+        <v>0.03242</v>
+      </c>
+      <c r="I73">
         <v>0.00715</v>
       </c>
     </row>

</xml_diff>